<commit_message>
ein paar kommentare hinzugefügt; Zeitblätter + Dokumentation der Sensorboard Library
</commit_message>
<xml_diff>
--- a/Zeitblätter/Tobias Breuß.xlsx
+++ b/Zeitblätter/Tobias Breuß.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ursus/Git/AlienHacky/Zeitblätter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Documents\AlienHacky\Zeitblätter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="51195" windowHeight="28260" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Oktober" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Dezember" sheetId="3" r:id="rId3"/>
     <sheet name="Jänner" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
     <t>Datum</t>
   </si>
@@ -46,11 +46,20 @@
   <si>
     <t>Zeitblatt: Tobias Breuß</t>
   </si>
+  <si>
+    <t>CCS zum Laufen bringen</t>
+  </si>
+  <si>
+    <t>CCS zum Laufen bringen; Gyro Sensor auslesen</t>
+  </si>
+  <si>
+    <t>Recherche Sensor Board</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
@@ -112,13 +121,44 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -391,18 +431,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="63.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="63.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -413,195 +453,195 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42644</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>A4+1</f>
         <v>42645</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A34" si="0">A5+1</f>
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>42647</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>42648</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>42649</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>42650</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>42651</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>42652</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>42653</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>42654</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>42655</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>42656</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>42657</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>42658</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>42659</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>42660</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>42661</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>42662</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>42663</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>42664</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>42665</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>42666</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>42667</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>42668</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>42669</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>42670</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>42671</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>42672</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>42673</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>42674</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
@@ -610,22 +650,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
   </sheetData>
@@ -639,17 +679,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="56.83203125" customWidth="1"/>
+    <col min="3" max="3" width="56.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -660,192 +700,192 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42675</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>A4+1</f>
         <v>42676</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A33" si="0">A5+1</f>
         <v>42677</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>42678</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>42679</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>42680</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>42681</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>42682</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>42683</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>42684</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>42685</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>42686</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>42687</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>42688</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>42689</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>42690</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>42691</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>42692</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>42693</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>42694</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>42695</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>42696</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>42697</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>42698</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>42699</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>42700</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>42701</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>42702</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>42703</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>42704</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
@@ -865,17 +905,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="61.33203125" customWidth="1"/>
+    <col min="3" max="3" width="61.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -886,195 +926,195 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>A4+1</f>
         <v>42706</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A34" si="0">A5+1</f>
         <v>42707</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>42708</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>42709</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>42710</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>42711</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>42712</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>42713</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>42714</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>42715</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>42716</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>42717</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>42718</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>42719</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>42720</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>42721</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>42722</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>42723</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>42724</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>42725</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>42726</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>42727</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>42728</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>42729</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>42730</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>42731</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>42732</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>42733</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>42734</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>42735</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
@@ -1092,19 +1132,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1115,201 +1157,219 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>42736</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42644</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>A4+1</f>
-        <v>42737</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42645</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A34" si="0">A5+1</f>
-        <v>42738</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42646</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
-        <v>42739</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
-        <v>42740</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42648</v>
+      </c>
+      <c r="B8">
+        <v>1.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
-        <v>42741</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42649</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
-        <v>42742</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42650</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
-        <v>42743</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42651</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
-        <v>42744</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42652</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
-        <v>42745</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42653</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
-        <v>42746</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42654</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
-        <v>42747</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42655</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
-        <v>42748</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42656</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
-        <v>42749</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42657</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
-        <v>42750</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42658</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
-        <v>42751</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42659</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
-        <v>42752</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42660</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
-        <v>42753</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42661</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
-        <v>42754</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42662</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
-        <v>42755</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
-        <v>42756</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42664</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
-        <v>42757</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42665</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
-        <v>42758</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
-        <v>42760</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
-        <v>42761</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
-        <v>42762</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42670</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
-        <v>42763</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+        <v>42671</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
-        <v>42764</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42672</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
-        <v>42765</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42673</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
-        <v>42766</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42674</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="2">
         <f>SUM(B5:B34)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funkmodul treibersuche; IAR muss wohl benutzt werden
</commit_message>
<xml_diff>
--- a/Zeitblätter/Tobias Breuß.xlsx
+++ b/Zeitblätter/Tobias Breuß.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t>Datum</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Gyro Auswertung</t>
+  </si>
+  <si>
+    <t>Funkmodul Treibersuche</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -555,6 +558,12 @@
         <f t="shared" si="0"/>
         <v>42654</v>
       </c>
+      <c r="B14">
+        <v>1.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -685,7 +694,7 @@
       </c>
       <c r="B36" s="2">
         <f>SUM(B4:B34)</f>
-        <v>18</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
neues Board beispiel; Remo-Ti API;
</commit_message>
<xml_diff>
--- a/Zeitblätter/Tobias Breuß.xlsx
+++ b/Zeitblätter/Tobias Breuß.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Documents\AlienSoccer\Zeitblätter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Documents\AlienHacky\Zeitblätter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>Datum</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>neues Funkmodul Recherche</t>
+  </si>
+  <si>
+    <t>neues Funkmodul Recherche; CCS Beispiel und API Guide</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -586,97 +589,103 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>42657</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>42658</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>42659</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1.5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>42660</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>42661</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>42662</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>42663</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>42664</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>42665</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>42666</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>42667</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>42668</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>42669</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>42670</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>42671</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>42672</v>
@@ -703,7 +712,7 @@
       </c>
       <c r="B36" s="2">
         <f>SUM(B4:B34)</f>
-        <v>21.5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Beispiele für Funkübertragung des neuen Boards hinzugefügt; Unterlagen über einen Latenztest hinzugefügt
</commit_message>
<xml_diff>
--- a/Zeitblätter/Tobias Breuß.xlsx
+++ b/Zeitblätter/Tobias Breuß.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>Datum</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>neues Funkmodul Recherche; CCS Beispiel und API Guide</t>
+  </si>
+  <si>
+    <t>neues Funkmodul Examples</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -618,6 +621,12 @@
         <f t="shared" si="0"/>
         <v>42660</v>
       </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -712,7 +721,7 @@
       </c>
       <c r="B36" s="2">
         <f>SUM(B4:B34)</f>
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
neues projekt "sensorhub_cc2560" i2c funktioniert nicht
</commit_message>
<xml_diff>
--- a/Zeitblätter/Tobias Breuß.xlsx
+++ b/Zeitblätter/Tobias Breuß.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Documents\AlienSoccer\Zeitblätter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Documents\AlienHacky\Zeitblätter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Datum</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Teammeeting + Funkmodul</t>
+  </si>
+  <si>
+    <t>Sensorboard auf neuem Modul</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -687,6 +690,12 @@
         <f t="shared" si="0"/>
         <v>42667</v>
       </c>
+      <c r="B27">
+        <v>4.5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -739,7 +748,7 @@
       </c>
       <c r="B36" s="2">
         <f>SUM(B4:B34)</f>
-        <v>30.5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>